<commit_message>
update cost and CI
</commit_message>
<xml_diff>
--- a/exposan/htl/data/impact_items_master_database_09052024.xlsx
+++ b/exposan/htl/data/impact_items_master_database_09052024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD_CEE/coding/cloned_packages/EXPOsan/exposan/htl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28DAD71-05F0-9E47-B314-07D8FE25D408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B96AE2-3DD0-E648-88DF-C77CAECB2095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20960" yWindow="8740" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="20600" yWindow="3900" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="137">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -416,6 +416,36 @@
   </si>
   <si>
     <t>need to estimate GWP for 70% solution</t>
+  </si>
+  <si>
+    <t>Natural_gas (superseded)</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>market for natural gas, low pressure</t>
+  </si>
+  <si>
+    <t>39 MJ/m3</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>market for carbon dioxide, in chemical industry</t>
+  </si>
+  <si>
+    <t>byproduct of ammonia production</t>
+  </si>
+  <si>
+    <t>byproduct of titanium sponge production</t>
+  </si>
+  <si>
+    <t>Liquid_CO2</t>
+  </si>
+  <si>
+    <t>market for carbon dioxide, liquid</t>
   </si>
 </sst>
 </file>
@@ -479,12 +509,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -500,7 +536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -508,7 +544,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -516,6 +551,12 @@
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -837,15 +878,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C13"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
@@ -854,13 +895,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1058,6 +1099,9 @@
       <c r="D14" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -1149,128 +1193,131 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2" t="s">
+    <row r="21" spans="1:5" s="14" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>76</v>
+        <v>28</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
+      <c r="C24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
     </row>
     <row r="26" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="C26" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
     </row>
     <row r="27" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>23</v>
@@ -1278,13 +1325,13 @@
     </row>
     <row r="30" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>23</v>
@@ -1292,13 +1339,13 @@
     </row>
     <row r="31" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>23</v>
@@ -1306,58 +1353,58 @@
     </row>
     <row r="32" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="33" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>74</v>
+        <v>23</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>23</v>
@@ -1365,214 +1412,259 @@
     </row>
     <row r="36" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>23</v>
+        <v>74</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>96</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>96</v>
+        <v>23</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C24:E24"/>
     <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1581,10 +1673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE2E960-887B-1E49-80AF-9619BDC224B9}">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1857,7 +1949,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="2">
-        <f>0.10261503/20+19/20*C26</f>
+        <f>0.10261503/20+19/20*C27</f>
         <v>5.5298725680000002E-3</v>
       </c>
       <c r="D11" s="2">
@@ -1883,7 +1975,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2">
-        <f>2.3210523*0.7+C26*0.3</f>
+        <f>2.3210523*0.7+C27*0.3</f>
         <v>1.6248626482319999</v>
       </c>
       <c r="D12" s="2">
@@ -2078,566 +2170,569 @@
       </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="2">
+    <row r="20" spans="1:14" s="15" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="14">
         <f>0.050399856*50</f>
         <v>2.5199927999999998</v>
       </c>
-      <c r="D20" s="2">
-        <f t="shared" ref="D20:D40" si="10">C20*0.9</f>
+      <c r="D20" s="14">
+        <f t="shared" ref="D20:D41" si="10">C20*0.9</f>
         <v>2.2679935200000001</v>
       </c>
-      <c r="E20" s="2">
-        <f t="shared" ref="E20:E40" si="11">C20*1.1</f>
+      <c r="E20" s="14">
+        <f t="shared" ref="E20:E41" si="11">C20*1.1</f>
         <v>2.77199208</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="7"/>
+      <c r="F20" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="18"/>
     </row>
     <row r="21" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.47016122999999999</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" ref="D21" si="12">C21*0.9</f>
+        <v>0.42314510700000002</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" ref="E21" si="13">C21*1.1</f>
+        <v>0.51717735300000001</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="2">
         <v>0.48748859</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D22" s="2">
         <f t="shared" si="10"/>
         <v>0.43873973100000002</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E22" s="2">
         <f t="shared" si="11"/>
         <v>0.53623744900000003</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="F22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2">
         <v>-0.44231485999999998</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D23" s="2">
         <f t="shared" si="10"/>
         <v>-0.39808337399999999</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E23" s="2">
         <f t="shared" si="11"/>
         <v>-0.48654634600000002</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="14"/>
-      <c r="N22" s="11"/>
-    </row>
-    <row r="23" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="F23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="N23" s="10"/>
+    </row>
+    <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="2">
-        <f>0.147*C39+0.1222*C37+87.3/3600*C40+2.3704*C39+0.312*C38+(1000-1000*7.8/100/101.07*207.43)/1000*C33+0.9454*C26+1000*7.8/100/1000*C34/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C35+0.487*1000*7.8/100/101.07*207.43/1000*C40+2.59/1000*C36</f>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2">
+        <f>0.147*C40+0.1222*C38+87.3/3600*C41+2.3704*C40+0.312*C39+(1000-1000*7.8/100/101.07*207.43)/1000*C34+0.9454*C27+1000*7.8/100/1000*C35/35335*2665+1000*7.8/100/101.07*(207.43-101.07)/1000*C36+0.487*1000*7.8/100/101.07*207.43/1000*C41+2.59/1000*C37</f>
         <v>471.09893696226777</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D24" s="2">
         <f t="shared" si="10"/>
         <v>423.98904326604099</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E24" s="2">
         <f t="shared" si="11"/>
         <v>518.20883065849455</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="F24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="2">
-        <f>0.4168*C38+3.358*C37+0.206*C39+1.6569*C39+0.4856*C38+0.0149*C40+1.2669*C38+0.7722*C25+0.6177*C26+0.0349*C27+0.136*C28+0.0834*C29+0.0973*C30+0.0088*C31+1.301*C32</f>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2">
+        <f>0.4168*C39+3.358*C38+0.206*C40+1.6569*C40+0.4856*C39+0.0149*C41+1.2669*C39+0.7722*C26+0.6177*C27+0.0349*C28+0.136*C29+0.0834*C30+0.0973*C31+0.0088*C32+1.301*C33</f>
         <v>5.9473882820744883</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <f t="shared" si="10"/>
         <v>5.3526494538670395</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <f t="shared" si="11"/>
         <v>6.5421271102819381</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="F25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2">
         <v>1.4810466</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D26" s="2">
         <f t="shared" si="10"/>
         <v>1.33294194</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E26" s="2">
         <f t="shared" si="11"/>
         <v>1.6291512600000002</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="F26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2">
         <v>4.2012743999999999E-4</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D27" s="2">
         <f t="shared" si="10"/>
         <v>3.7811469600000002E-4</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E27" s="2">
         <f t="shared" si="11"/>
         <v>4.6214018400000001E-4</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="2">
         <v>1.3560825000000001</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D28" s="2">
         <f t="shared" si="10"/>
         <v>1.2204742500000001</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E28" s="2">
         <f t="shared" si="11"/>
         <v>1.4916907500000003</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="F28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="2">
         <v>7.9620949000000003</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D29" s="2">
         <f t="shared" si="10"/>
         <v>7.1658854100000005</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E29" s="2">
         <f t="shared" si="11"/>
         <v>8.758304390000001</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K28" s="8"/>
-    </row>
-    <row r="29" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="F29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="2">
         <v>30.095762000000001</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D30" s="2">
         <f t="shared" si="10"/>
         <v>27.086185800000003</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E30" s="2">
         <f t="shared" si="11"/>
         <v>33.105338200000006</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="F30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="2">
         <v>0.12410437000000001</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D31" s="2">
         <f t="shared" si="10"/>
         <v>0.11169393300000001</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E31" s="2">
         <f t="shared" si="11"/>
         <v>0.13651480700000002</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="F31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="2">
+      <c r="B32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="2">
         <v>1.5621537000000001</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <f t="shared" si="10"/>
         <v>1.4059383300000001</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E32" s="2">
         <f t="shared" si="11"/>
         <v>1.7183690700000003</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="F32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="2">
+      <c r="B33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2">
         <v>0.46772893999999998</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D33" s="2">
         <f t="shared" si="10"/>
         <v>0.42095604599999997</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E33" s="2">
         <f t="shared" si="11"/>
         <v>0.51450183400000005</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N32" s="9"/>
-    </row>
-    <row r="33" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="F33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="8"/>
+    </row>
+    <row r="34" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="2">
+      <c r="B34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="2">
         <v>3.2395651999999999</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D34" s="2">
         <f t="shared" si="10"/>
         <v>2.9156086800000001</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E34" s="2">
         <f t="shared" si="11"/>
         <v>3.5635217200000002</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N33" s="9"/>
-    </row>
-    <row r="34" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="F34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N34" s="8"/>
+    </row>
+    <row r="35" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="2">
+      <c r="B35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="2">
         <v>79553.031000000003</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D35" s="2">
         <f t="shared" si="10"/>
         <v>71597.727899999998</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E35" s="2">
         <f t="shared" si="11"/>
         <v>87508.334100000007</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N34" s="9"/>
-    </row>
-    <row r="35" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="F35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N35" s="8"/>
+    </row>
+    <row r="36" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="2">
+      <c r="B36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="2">
         <v>0.58090182000000001</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D36" s="2">
         <f t="shared" si="10"/>
         <v>0.52281163800000008</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E36" s="2">
         <f t="shared" si="11"/>
         <v>0.63899200200000006</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="4"/>
-    </row>
-    <row r="36" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="F36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="4"/>
+    </row>
+    <row r="37" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="2">
+      <c r="B37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2">
         <v>0.21777796999999999</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D37" s="2">
         <f t="shared" si="10"/>
         <v>0.196000173</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E37" s="2">
         <f t="shared" si="11"/>
         <v>0.239555767</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="F37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="2">
+      <c r="B38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2">
         <v>6.5877932E-2</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D38" s="2">
         <f t="shared" si="10"/>
         <v>5.9290138800000003E-2</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E38" s="2">
         <f t="shared" si="11"/>
         <v>7.2465725200000011E-2</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O37" s="10"/>
-    </row>
-    <row r="38" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="F38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" s="9"/>
+    </row>
+    <row r="39" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="2">
+      <c r="B39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2">
         <v>5.0399856E-2</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D39" s="2">
         <f t="shared" si="10"/>
         <v>4.5359870400000002E-2</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E39" s="2">
         <f t="shared" si="11"/>
         <v>5.5439841600000005E-2</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="F39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="2">
+      <c r="B40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2">
         <v>0.10261104</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D40" s="2">
         <f t="shared" si="10"/>
         <v>9.2349936000000007E-2</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E40" s="2">
         <f t="shared" si="11"/>
         <v>0.11287214400000001</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="F40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="2">
+      <c r="B41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2">
         <v>0.48748859</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D41" s="2">
         <f t="shared" si="10"/>
         <v>0.43873973100000002</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E41" s="2">
         <f t="shared" si="11"/>
         <v>0.53623744900000003</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="2">
-        <v>-0.33231451000000001</v>
-      </c>
-      <c r="D41" s="2">
-        <f t="shared" ref="D41" si="12">C41*0.9</f>
-        <v>-0.29908305900000004</v>
-      </c>
-      <c r="E41" s="2">
-        <f t="shared" ref="E41" si="13">C41*1.1</f>
-        <v>-0.36554596100000003</v>
-      </c>
       <c r="F41" s="2" t="s">
         <v>1</v>
       </c>
@@ -2647,21 +2742,21 @@
     </row>
     <row r="42" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="2">
-        <v>0.13004958</v>
+        <v>-0.33231451000000001</v>
       </c>
       <c r="D42" s="2">
         <f t="shared" ref="D42" si="14">C42*0.9</f>
-        <v>0.117044622</v>
+        <v>-0.29908305900000004</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" ref="E42" si="15">C42*1.1</f>
-        <v>0.14305453800000001</v>
+        <v>-0.36554596100000003</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>1</v>
@@ -2672,21 +2767,21 @@
     </row>
     <row r="43" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="2">
-        <v>0.22290007000000001</v>
+        <v>0.13004958</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" ref="D43:D44" si="16">C43*0.9</f>
-        <v>0.20061006300000001</v>
+        <f t="shared" ref="D43" si="16">C43*0.9</f>
+        <v>0.117044622</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" ref="E43:E44" si="17">C43*1.1</f>
-        <v>0.24519007700000003</v>
+        <f t="shared" ref="E43" si="17">C43*1.1</f>
+        <v>0.14305453800000001</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>1</v>
@@ -2697,21 +2792,21 @@
     </row>
     <row r="44" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C44" s="2">
-        <v>8.2744841E-3</v>
+        <v>0.22290007000000001</v>
       </c>
       <c r="D44" s="2">
-        <f t="shared" si="16"/>
-        <v>7.4470356900000001E-3</v>
+        <f t="shared" ref="D44:D47" si="18">C44*0.9</f>
+        <v>0.20061006300000001</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="17"/>
-        <v>9.1019325100000006E-3</v>
+        <f t="shared" ref="E44:E47" si="19">C44*1.1</f>
+        <v>0.24519007700000003</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>1</v>
@@ -2722,172 +2817,245 @@
     </row>
     <row r="45" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="2">
+        <v>8.2744841E-3</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="18"/>
+        <v>7.4470356900000001E-3</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="19"/>
+        <v>9.1019325100000006E-3</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.66136795000000004</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" ref="D46" si="20">C46*0.9</f>
+        <v>0.59523115500000001</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" ref="E46" si="21">C46*1.1</f>
+        <v>0.72750474500000006</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="2">
+      <c r="B48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="2">
         <v>1.4566920000000001</v>
       </c>
-      <c r="D45" s="2">
-        <f t="shared" ref="D45" si="18">C45*0.9</f>
+      <c r="D48" s="2">
+        <f t="shared" ref="D48" si="22">C48*0.9</f>
         <v>1.3110228000000002</v>
       </c>
-      <c r="E45" s="2">
-        <f t="shared" ref="E45" si="19">C45*1.1</f>
+      <c r="E48" s="2">
+        <f t="shared" ref="E48" si="23">C48*1.1</f>
         <v>1.6023612000000003</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="F48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="2">
+      <c r="B49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="2">
         <v>2.4833471999999999</v>
       </c>
-      <c r="D46" s="2">
-        <f t="shared" ref="D46:D48" si="20">C46*0.9</f>
+      <c r="D49" s="2">
+        <f t="shared" ref="D49:D51" si="24">C49*0.9</f>
         <v>2.23501248</v>
       </c>
-      <c r="E46" s="2">
-        <f t="shared" ref="E46:E48" si="21">C46*1.1</f>
+      <c r="E49" s="2">
+        <f t="shared" ref="E49:E51" si="25">C49*1.1</f>
         <v>2.7316819200000002</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="F49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="2">
+      <c r="B50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="2">
         <v>1.2510711000000001</v>
       </c>
-      <c r="D47" s="2">
-        <f t="shared" si="20"/>
+      <c r="D50" s="2">
+        <f t="shared" si="24"/>
         <v>1.12596399</v>
       </c>
-      <c r="E47" s="2">
-        <f t="shared" si="21"/>
+      <c r="E50" s="2">
+        <f t="shared" si="25"/>
         <v>1.3761782100000002</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N47" s="9"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="F50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N50" s="8"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="2">
+      <c r="B51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="2">
         <v>1.6799470999999999</v>
       </c>
-      <c r="D48" s="2">
-        <f t="shared" si="20"/>
+      <c r="D51" s="2">
+        <f t="shared" si="24"/>
         <v>1.51195239</v>
       </c>
-      <c r="E48" s="2">
-        <f t="shared" si="21"/>
+      <c r="E51" s="2">
+        <f t="shared" si="25"/>
         <v>1.84794181</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="7:19" x14ac:dyDescent="0.2">
-      <c r="K49" s="12"/>
-      <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-      <c r="O49" s="12"/>
-      <c r="P49" s="12"/>
-      <c r="Q49" s="12"/>
-      <c r="R49" s="12"/>
-      <c r="S49" s="12"/>
-    </row>
-    <row r="50" spans="7:19" x14ac:dyDescent="0.2">
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-      <c r="O50" s="12"/>
-      <c r="P50" s="12"/>
-      <c r="Q50" s="12"/>
-      <c r="R50" s="12"/>
-      <c r="S50" s="12"/>
-    </row>
-    <row r="51" spans="7:19" x14ac:dyDescent="0.2">
-      <c r="K51" s="12"/>
-      <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
-      <c r="R51" s="12"/>
-      <c r="S51" s="12"/>
-    </row>
-    <row r="53" spans="7:19" x14ac:dyDescent="0.2">
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="12"/>
-      <c r="R53" s="12"/>
-      <c r="S53" s="12"/>
-    </row>
-    <row r="55" spans="7:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="G55" s="5"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="13"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="13"/>
-      <c r="O55" s="13"/>
-      <c r="P55" s="13"/>
-      <c r="Q55" s="13"/>
-      <c r="R55" s="13"/>
-      <c r="S55" s="13"/>
-    </row>
-    <row r="58" spans="7:19" x14ac:dyDescent="0.2">
-      <c r="N58" s="6"/>
-    </row>
-    <row r="59" spans="7:19" x14ac:dyDescent="0.2">
-      <c r="N59" s="6"/>
-    </row>
-    <row r="60" spans="7:19" x14ac:dyDescent="0.2">
-      <c r="N60" s="6"/>
-    </row>
-    <row r="61" spans="7:19" x14ac:dyDescent="0.2">
+      <c r="F51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="11"/>
+      <c r="S52" s="11"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="Q54" s="11"/>
+      <c r="R54" s="11"/>
+      <c r="S54" s="11"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+    </row>
+    <row r="58" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="G58" s="5"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="12"/>
+      <c r="S58" s="12"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="N61" s="6"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N62" s="6"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N63" s="6"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="N64" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>